<commit_message>
fixed quad transceiver footprint + reduce led brightness
</commit_message>
<xml_diff>
--- a/EDA/SMT/quack-all-pos.xlsx
+++ b/EDA/SMT/quack-all-pos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="84">
   <si>
     <t>quack-all-pos</t>
   </si>
@@ -34,10 +34,10 @@
     <t>C1</t>
   </si>
   <si>
-    <t>136.2225mm</t>
-  </si>
-  <si>
-    <t>-95.2500mm</t>
+    <t>136.5625mm</t>
+  </si>
+  <si>
+    <t>-95.5000mm</t>
   </si>
   <si>
     <t>Top</t>
@@ -73,6 +73,33 @@
     <t>-101.0625mm</t>
   </si>
   <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>174.0000mm</t>
+  </si>
+  <si>
+    <t>-99.0000mm</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>-93.0500mm</t>
+  </si>
+  <si>
+    <t>C8</t>
+  </si>
+  <si>
+    <t>-108.0000mm</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>167.0000mm</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
@@ -112,6 +139,12 @@
     <t>IC2</t>
   </si>
   <si>
+    <t>168.5000mm</t>
+  </si>
+  <si>
+    <t>-95.0000mm</t>
+  </si>
+  <si>
     <t>R1</t>
   </si>
   <si>
@@ -157,6 +190,15 @@
     <t>-101.6000mm</t>
   </si>
   <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>170.0500mm</t>
+  </si>
+  <si>
+    <t>-110.0000mm</t>
+  </si>
+  <si>
     <t>FB1</t>
   </si>
   <si>
@@ -166,9 +208,6 @@
     <t>FB2</t>
   </si>
   <si>
-    <t>167.0000mm</t>
-  </si>
-  <si>
     <t>FB3</t>
   </si>
   <si>
@@ -188,9 +227,6 @@
   </si>
   <si>
     <t>FB5</t>
-  </si>
-  <si>
-    <t>174.0000mm</t>
   </si>
   <si>
     <t>-78.5000mm</t>
@@ -1515,7 +1551,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E29"/>
+  <dimension ref="A2:E34"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1651,7 +1687,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="11">
-        <v>180</v>
+        <v>270</v>
       </c>
       <c r="E8" t="s" s="10">
         <v>9</v>
@@ -1662,13 +1698,13 @@
         <v>23</v>
       </c>
       <c r="B9" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s" s="10">
         <v>24</v>
       </c>
-      <c r="C9" t="s" s="10">
-        <v>22</v>
-      </c>
       <c r="D9" s="11">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E9" t="s" s="10">
         <v>9</v>
@@ -1679,13 +1715,13 @@
         <v>25</v>
       </c>
       <c r="B10" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s" s="10">
         <v>26</v>
       </c>
-      <c r="C10" t="s" s="10">
-        <v>22</v>
-      </c>
       <c r="D10" s="11">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E10" t="s" s="10">
         <v>9</v>
@@ -1699,10 +1735,10 @@
         <v>28</v>
       </c>
       <c r="C11" t="s" s="10">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D11" s="11">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E11" t="s" s="10">
         <v>9</v>
@@ -1719,7 +1755,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="11">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="E12" t="s" s="10">
         <v>9</v>
@@ -1730,13 +1766,13 @@
         <v>32</v>
       </c>
       <c r="B13" t="s" s="9">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s" s="10">
         <v>31</v>
       </c>
       <c r="D13" s="11">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E13" t="s" s="10">
         <v>9</v>
@@ -1744,16 +1780,16 @@
     </row>
     <row r="14" ht="20.05" customHeight="1">
       <c r="A14" t="s" s="8">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s" s="9">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s" s="10">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D14" s="11">
-        <v>270</v>
+        <v>180</v>
       </c>
       <c r="E14" t="s" s="10">
         <v>9</v>
@@ -1767,10 +1803,10 @@
         <v>37</v>
       </c>
       <c r="C15" t="s" s="10">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="11">
-        <v>270</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s" s="10">
         <v>9</v>
@@ -1778,13 +1814,13 @@
     </row>
     <row r="16" ht="20.05" customHeight="1">
       <c r="A16" t="s" s="8">
+        <v>38</v>
+      </c>
+      <c r="B16" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="B16" t="s" s="9">
+      <c r="C16" t="s" s="10">
         <v>40</v>
-      </c>
-      <c r="C16" t="s" s="10">
-        <v>38</v>
       </c>
       <c r="D16" s="11">
         <v>270</v>
@@ -1801,10 +1837,10 @@
         <v>42</v>
       </c>
       <c r="C17" t="s" s="10">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="D17" s="11">
-        <v>90</v>
+        <v>180</v>
       </c>
       <c r="E17" t="s" s="10">
         <v>9</v>
@@ -1812,13 +1848,13 @@
     </row>
     <row r="18" ht="20.05" customHeight="1">
       <c r="A18" t="s" s="8">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B18" t="s" s="9">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s" s="10">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D18" s="11">
         <v>270</v>
@@ -1829,16 +1865,16 @@
     </row>
     <row r="19" ht="20.05" customHeight="1">
       <c r="A19" t="s" s="8">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B19" t="s" s="9">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s" s="10">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D19" s="11">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E19" t="s" s="10">
         <v>9</v>
@@ -1846,16 +1882,16 @@
     </row>
     <row r="20" ht="20.05" customHeight="1">
       <c r="A20" t="s" s="8">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s" s="9">
+        <v>51</v>
+      </c>
+      <c r="C20" t="s" s="10">
         <v>49</v>
       </c>
-      <c r="C20" t="s" s="10">
-        <v>38</v>
-      </c>
-      <c r="D20" s="12">
-        <v>90</v>
+      <c r="D20" s="11">
+        <v>270</v>
       </c>
       <c r="E20" t="s" s="10">
         <v>9</v>
@@ -1863,15 +1899,15 @@
     </row>
     <row r="21" ht="20.05" customHeight="1">
       <c r="A21" t="s" s="8">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s" s="9">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s" s="10">
-        <v>38</v>
-      </c>
-      <c r="D21" s="12">
+        <v>46</v>
+      </c>
+      <c r="D21" s="11">
         <v>90</v>
       </c>
       <c r="E21" t="s" s="10">
@@ -1880,16 +1916,16 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="8">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s" s="9">
-        <v>53</v>
+        <v>17</v>
       </c>
       <c r="C22" t="s" s="10">
-        <v>54</v>
-      </c>
-      <c r="D22" s="12">
-        <v>0</v>
+        <v>55</v>
+      </c>
+      <c r="D22" s="11">
+        <v>270</v>
       </c>
       <c r="E22" t="s" s="10">
         <v>9</v>
@@ -1897,16 +1933,16 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s" s="9">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s" s="10">
-        <v>57</v>
-      </c>
-      <c r="D23" s="12">
-        <v>90</v>
+        <v>58</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0</v>
       </c>
       <c r="E23" t="s" s="10">
         <v>9</v>
@@ -1914,16 +1950,16 @@
     </row>
     <row r="24" ht="20.05" customHeight="1">
       <c r="A24" t="s" s="8">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s" s="9">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s" s="10">
-        <v>60</v>
-      </c>
-      <c r="D24" s="12">
-        <v>0</v>
+        <v>61</v>
+      </c>
+      <c r="D24" s="11">
+        <v>270</v>
       </c>
       <c r="E24" t="s" s="10">
         <v>9</v>
@@ -1931,16 +1967,16 @@
     </row>
     <row r="25" ht="20.05" customHeight="1">
       <c r="A25" t="s" s="8">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s" s="9">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s" s="10">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="D25" s="12">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E25" t="s" s="10">
         <v>9</v>
@@ -1948,16 +1984,16 @@
     </row>
     <row r="26" ht="20.05" customHeight="1">
       <c r="A26" t="s" s="8">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B26" t="s" s="9">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="C26" t="s" s="10">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D26" s="12">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s" s="10">
         <v>9</v>
@@ -1968,10 +2004,10 @@
         <v>65</v>
       </c>
       <c r="B27" t="s" s="9">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C27" t="s" s="10">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D27" s="12">
         <v>0</v>
@@ -1982,16 +2018,16 @@
     </row>
     <row r="28" ht="20.05" customHeight="1">
       <c r="A28" t="s" s="8">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B28" t="s" s="9">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s" s="10">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D28" s="12">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s" s="10">
         <v>9</v>
@@ -1999,18 +2035,103 @@
     </row>
     <row r="29" ht="20.05" customHeight="1">
       <c r="A29" t="s" s="8">
+        <v>71</v>
+      </c>
+      <c r="B29" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s" s="10">
+        <v>72</v>
+      </c>
+      <c r="D29" s="12">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" ht="20.05" customHeight="1">
+      <c r="A30" t="s" s="8">
+        <v>73</v>
+      </c>
+      <c r="B30" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="C30" t="s" s="10">
+        <v>74</v>
+      </c>
+      <c r="D30" s="12">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" ht="20.05" customHeight="1">
+      <c r="A31" t="s" s="8">
+        <v>75</v>
+      </c>
+      <c r="B31" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s" s="10">
+        <v>76</v>
+      </c>
+      <c r="D31" s="12">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" ht="20.05" customHeight="1">
+      <c r="A32" t="s" s="8">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s" s="9">
+        <v>21</v>
+      </c>
+      <c r="C32" t="s" s="10">
+        <v>78</v>
+      </c>
+      <c r="D32" s="12">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" ht="20.05" customHeight="1">
+      <c r="A33" t="s" s="8">
+        <v>79</v>
+      </c>
+      <c r="B33" t="s" s="9">
+        <v>80</v>
+      </c>
+      <c r="C33" t="s" s="10">
+        <v>81</v>
+      </c>
+      <c r="D33" s="12">
+        <v>0</v>
+      </c>
+      <c r="E33" t="s" s="10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" ht="20.05" customHeight="1">
+      <c r="A34" t="s" s="8">
+        <v>82</v>
+      </c>
+      <c r="B34" t="s" s="9">
+        <v>83</v>
+      </c>
+      <c r="C34" t="s" s="10">
         <v>70</v>
       </c>
-      <c r="B29" t="s" s="9">
-        <v>71</v>
-      </c>
-      <c r="C29" t="s" s="10">
-        <v>57</v>
-      </c>
-      <c r="D29" s="11">
+      <c r="D34" s="11">
         <v>270</v>
       </c>
-      <c r="E29" t="s" s="10">
+      <c r="E34" t="s" s="10">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed some SMT positions for pick and place
</commit_message>
<xml_diff>
--- a/EDA/SMT/quack-all-pos.xlsx
+++ b/EDA/SMT/quack-all-pos.xlsx
@@ -79,7 +79,7 @@
     <t>174.0000mm</t>
   </si>
   <si>
-    <t>-99.0000mm</t>
+    <t>-97.0000mm</t>
   </si>
   <si>
     <t>C7</t>
@@ -166,7 +166,7 @@
     <t>R2</t>
   </si>
   <si>
-    <t>172.0000mm</t>
+    <t>169.0000mm</t>
   </si>
   <si>
     <t>-119.0625mm</t>
@@ -175,7 +175,10 @@
     <t>R3</t>
   </si>
   <si>
-    <t>174.5000mm</t>
+    <t>171.5000mm</t>
+  </si>
+  <si>
+    <t>-119.0000mm</t>
   </si>
   <si>
     <t>R4</t>
@@ -187,9 +190,6 @@
     <t>R5</t>
   </si>
   <si>
-    <t>-97.0000mm</t>
-  </si>
-  <si>
     <t>R6</t>
   </si>
   <si>
@@ -223,16 +223,16 @@
     <t>FB2</t>
   </si>
   <si>
-    <t>167.0000mm</t>
+    <t>155.5000mm</t>
+  </si>
+  <si>
+    <t>-111.5000mm</t>
   </si>
   <si>
     <t>FB3</t>
   </si>
   <si>
-    <t>154.0625mm</t>
-  </si>
-  <si>
-    <t>-110.5000mm</t>
+    <t>153.0000mm</t>
   </si>
   <si>
     <t>FB4</t>
@@ -1923,7 +1923,7 @@
         <v>54</v>
       </c>
       <c r="C21" t="s" s="10">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D21" s="11">
         <v>270</v>
@@ -1934,10 +1934,10 @@
     </row>
     <row r="22" ht="20.05" customHeight="1">
       <c r="A22" t="s" s="8">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s" s="9">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s" s="10">
         <v>49</v>
@@ -1951,13 +1951,13 @@
     </row>
     <row r="23" ht="20.05" customHeight="1">
       <c r="A23" t="s" s="8">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s" s="9">
         <v>17</v>
       </c>
       <c r="C23" t="s" s="10">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="D23" s="11">
         <v>270</v>
@@ -1974,7 +1974,7 @@
         <v>26</v>
       </c>
       <c r="C24" t="s" s="10">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="D24" s="11">
         <v>90</v>
@@ -1991,7 +1991,7 @@
         <v>61</v>
       </c>
       <c r="C25" t="s" s="10">
-        <v>58</v>
+        <v>22</v>
       </c>
       <c r="D25" s="11">
         <v>90</v>
@@ -2059,7 +2059,7 @@
         <v>70</v>
       </c>
       <c r="C29" t="s" s="10">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D29" s="12">
         <v>90</v>
@@ -2070,16 +2070,16 @@
     </row>
     <row r="30" ht="20.05" customHeight="1">
       <c r="A30" t="s" s="8">
+        <v>72</v>
+      </c>
+      <c r="B30" t="s" s="9">
+        <v>73</v>
+      </c>
+      <c r="C30" t="s" s="10">
         <v>71</v>
       </c>
-      <c r="B30" t="s" s="9">
-        <v>72</v>
-      </c>
-      <c r="C30" t="s" s="10">
-        <v>73</v>
-      </c>
       <c r="D30" s="12">
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="E30" t="s" s="10">
         <v>9</v>

</xml_diff>